<commit_message>
added final test pipeline notebook and new supervised model plus refactoring of xl files
</commit_message>
<xml_diff>
--- a/DealMatch/targets_clean_test.xlsx
+++ b/DealMatch/targets_clean_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelbroza/code/michabrz/DealMatch/DealMatch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{377156F1-4877-7946-8320-135F856E06F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CAD82A-19EC-0F4E-9EE8-6DD1DCCF0699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33300" yWindow="-1060" windowWidth="30240" windowHeight="17800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>deal_id</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t>1303 Sonne</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Bavaria</t>
   </si>
 </sst>
 </file>
@@ -490,7 +496,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -564,6 +570,12 @@
       <c r="I2">
         <v>3</v>
       </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
       <c r="L2" t="s">
         <v>13</v>
       </c>

</xml_diff>